<commit_message>
small updates to profiling
</commit_message>
<xml_diff>
--- a/performance-measurements.xlsx
+++ b/performance-measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomhultonharrop/Documents/Projects/cpp-remove-entities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73E80504-ACDE-674E-BF8D-1458DC7E936D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC37BB8E-B2B8-FD49-8652-D02A68B5A7DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16480" xr2:uid="{9350DD4D-C0D7-D049-86EC-11D23DCA51E7}"/>
   </bookViews>
@@ -304,22 +304,25 @@
                   <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76400000000000001</c:v>
+                  <c:v>0.73099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.49</c:v>
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.57</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7</c:v>
+                  <c:v>1.74</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.38</c:v>
+                  <c:v>1.34</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.52</c:v>
+                  <c:v>1.57</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>1.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1495,22 +1498,25 @@
                   <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76400000000000001</c:v>
+                  <c:v>0.73099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.49</c:v>
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.57</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7</c:v>
+                  <c:v>1.74</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.38</c:v>
+                  <c:v>1.34</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.52</c:v>
+                  <c:v>1.57</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>1.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3364,8 +3370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CABD1E-E4DF-164D-8791-5A9D183EC259}">
   <dimension ref="B2:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3503,22 +3509,25 @@
         <v>0.44</v>
       </c>
       <c r="H6">
-        <v>0.76400000000000001</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="I6">
-        <v>1.49</v>
+        <v>1.43</v>
+      </c>
+      <c r="J6">
+        <v>1.57</v>
       </c>
       <c r="K6">
-        <v>1.7</v>
+        <v>1.74</v>
       </c>
       <c r="L6">
-        <v>1.38</v>
+        <v>1.34</v>
       </c>
       <c r="M6">
-        <v>1.52</v>
+        <v>1.57</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">

</xml_diff>